<commit_message>
Adding more code for plotting
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -69,12 +70,18 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Yield</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,11 +426,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,4 +589,137 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C97F40D-5FCB-4C9D-85A4-97B46DEAC0D8}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1.45</v>
+      </c>
+      <c r="C2">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="C3">
+        <v>4.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3.12</v>
+      </c>
+      <c r="C4">
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4.13</v>
+      </c>
+      <c r="C5">
+        <v>8.1199999999999992</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5.67</v>
+      </c>
+      <c r="C6">
+        <v>10.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6.86</v>
+      </c>
+      <c r="C7">
+        <v>11.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7.52</v>
+      </c>
+      <c r="C8">
+        <v>15.07</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>8.32</v>
+      </c>
+      <c r="C9">
+        <v>16.559999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="C10">
+        <v>17.86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>10.34</v>
+      </c>
+      <c r="C11">
+        <v>21.09</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>